<commit_message>
finished refactoring heuristics to single classes for each of them
</commit_message>
<xml_diff>
--- a/src/main/java/net/clementlevallois/umigon/heuristics/resources/fr/fr.xlsx
+++ b/src/main/java/net/clementlevallois/umigon/heuristics/resources/fr/fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levallois\Google Drive\open\UmigonLambda\umigon-heuristics\src\main\java\net\clementlevallois\umigon\heuristics\resources\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703CD801-1F9F-4358-BE2A-105FA1B56B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233A9DE1-6BFE-4136-A17D-22EDEC49B22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_positive tone" sheetId="1" r:id="rId1"/>
@@ -15399,8 +15399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C871"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A378" sqref="A378"/>
+    <sheetView topLeftCell="A364" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23271,8 +23271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>